<commit_message>
Completed data for lab 1
</commit_message>
<xml_diff>
--- a/Lab 1 - Results Template.xlsx
+++ b/Lab 1 - Results Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mines0-my.sharepoint.com/personal/tessahaws_mines_edu/Documents/Years/Senior/Fall/Robotics/Labs/IntroToRobotics/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="331" documentId="8_{2817B20B-292F-46DE-8733-EDFD4BC374F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{356C3D19-B8D7-464F-8730-E7FD5A2B479D}"/>
+  <xr:revisionPtr revIDLastSave="431" documentId="8_{2817B20B-292F-46DE-8733-EDFD4BC374F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{160129E4-CFB6-4CA7-998F-33A732F52DA8}"/>
   <bookViews>
-    <workbookView xWindow="11442" yWindow="0" windowWidth="11676" windowHeight="13038" xr2:uid="{EA4EB6AE-EF90-46D8-9FD0-3C84C7D17E0F}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13152" xr2:uid="{EA4EB6AE-EF90-46D8-9FD0-3C84C7D17E0F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -553,7 +553,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="43">
   <si>
     <t>Radius of Pulley Wheel (m):</t>
   </si>
@@ -706,6 +706,9 @@
   </si>
   <si>
     <t>dark grey</t>
+  </si>
+  <si>
+    <t>*Using 255 PWM</t>
   </si>
 </sst>
 </file>
@@ -1004,7 +1007,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -1045,6 +1048,41 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1081,42 +1119,6 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2850,10 +2852,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F80C9C28-A187-4D77-9D7A-490A5A1079C7}">
-  <dimension ref="A1:AX35"/>
+  <dimension ref="A1:AX36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G8" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K23" sqref="K23"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2868,93 +2870,98 @@
     <col min="14" max="14" width="13.578125" customWidth="1"/>
     <col min="15" max="16" width="11.83984375" customWidth="1"/>
     <col min="17" max="17" width="13.26171875" customWidth="1"/>
+    <col min="19" max="19" width="13.83984375" customWidth="1"/>
+    <col min="20" max="20" width="11.734375" customWidth="1"/>
     <col min="23" max="23" width="14.83984375" customWidth="1"/>
     <col min="24" max="24" width="16.15625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:50" ht="20.399999999999999" x14ac:dyDescent="0.75">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="39" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="46"/>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
     </row>
     <row r="2" spans="1:50" ht="20.399999999999999" x14ac:dyDescent="0.75">
-      <c r="A2" s="46" t="s">
+      <c r="A2" s="39" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="46"/>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="46"/>
+      <c r="B2" s="39"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
     </row>
     <row r="4" spans="1:50" ht="81.599999999999994" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B4" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="D4" s="50" t="s">
+      <c r="D4" s="43" t="s">
         <v>34</v>
       </c>
-      <c r="E4" s="51"/>
-      <c r="F4" s="51"/>
-      <c r="G4" s="51"/>
-      <c r="H4" s="52"/>
-      <c r="J4" s="50" t="s">
+      <c r="E4" s="44"/>
+      <c r="F4" s="44"/>
+      <c r="G4" s="44"/>
+      <c r="H4" s="45"/>
+      <c r="J4" s="43" t="s">
         <v>35</v>
       </c>
-      <c r="K4" s="51"/>
-      <c r="L4" s="51"/>
-      <c r="M4" s="51"/>
-      <c r="N4" s="52"/>
-      <c r="P4" s="50" t="s">
+      <c r="K4" s="44"/>
+      <c r="L4" s="44"/>
+      <c r="M4" s="44"/>
+      <c r="N4" s="45"/>
+      <c r="P4" s="43" t="s">
         <v>36</v>
       </c>
-      <c r="Q4" s="51"/>
-      <c r="R4" s="51"/>
-      <c r="S4" s="51"/>
-      <c r="T4" s="51"/>
-      <c r="U4" s="51"/>
-      <c r="V4" s="52"/>
+      <c r="Q4" s="44"/>
+      <c r="R4" s="44"/>
+      <c r="S4" s="44"/>
+      <c r="T4" s="44"/>
+      <c r="U4" s="44"/>
+      <c r="V4" s="45"/>
     </row>
     <row r="6" spans="1:50" ht="23.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B6" s="53" t="s">
+      <c r="B6" s="46" t="s">
         <v>39</v>
       </c>
       <c r="K6" t="s">
         <v>40</v>
       </c>
+      <c r="W6" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="7" spans="1:50" ht="29.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="B7" s="54"/>
-      <c r="E7" s="47" t="s">
+      <c r="B7" s="47"/>
+      <c r="E7" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="F7" s="49"/>
-      <c r="G7" s="49"/>
-      <c r="H7" s="49"/>
-      <c r="I7" s="49"/>
-      <c r="J7" s="49"/>
-      <c r="K7" s="49"/>
-      <c r="L7" s="49"/>
-      <c r="M7" s="49"/>
-      <c r="N7" s="49"/>
-      <c r="O7" s="49"/>
-      <c r="P7" s="49"/>
-      <c r="Q7" s="48"/>
-      <c r="S7" s="43" t="s">
+      <c r="F7" s="42"/>
+      <c r="G7" s="42"/>
+      <c r="H7" s="42"/>
+      <c r="I7" s="42"/>
+      <c r="J7" s="42"/>
+      <c r="K7" s="42"/>
+      <c r="L7" s="42"/>
+      <c r="M7" s="42"/>
+      <c r="N7" s="42"/>
+      <c r="O7" s="42"/>
+      <c r="P7" s="42"/>
+      <c r="Q7" s="41"/>
+      <c r="S7" s="58" t="s">
         <v>24</v>
       </c>
-      <c r="T7" s="45"/>
-      <c r="U7" s="44"/>
-      <c r="W7" s="43" t="s">
+      <c r="T7" s="60"/>
+      <c r="U7" s="59"/>
+      <c r="W7" s="58" t="s">
         <v>29</v>
       </c>
-      <c r="X7" s="44"/>
+      <c r="X7" s="59"/>
     </row>
     <row r="8" spans="1:50" ht="28.9" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B8" s="55"/>
+      <c r="B8" s="48"/>
       <c r="E8" s="10" t="s">
         <v>27</v>
       </c>
@@ -3009,22 +3016,22 @@
       <c r="X8" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="AK8" s="34" t="s">
+      <c r="AK8" s="49" t="s">
         <v>16</v>
       </c>
-      <c r="AL8" s="35"/>
-      <c r="AM8" s="35"/>
-      <c r="AN8" s="35"/>
-      <c r="AO8" s="35"/>
-      <c r="AP8" s="36"/>
-      <c r="AS8" s="34" t="s">
+      <c r="AL8" s="50"/>
+      <c r="AM8" s="50"/>
+      <c r="AN8" s="50"/>
+      <c r="AO8" s="50"/>
+      <c r="AP8" s="51"/>
+      <c r="AS8" s="49" t="s">
         <v>17</v>
       </c>
-      <c r="AT8" s="35"/>
-      <c r="AU8" s="35"/>
-      <c r="AV8" s="35"/>
-      <c r="AW8" s="35"/>
-      <c r="AX8" s="36"/>
+      <c r="AT8" s="50"/>
+      <c r="AU8" s="50"/>
+      <c r="AV8" s="50"/>
+      <c r="AW8" s="50"/>
+      <c r="AX8" s="51"/>
     </row>
     <row r="9" spans="1:50" x14ac:dyDescent="0.55000000000000004">
       <c r="E9" s="11">
@@ -3079,34 +3086,36 @@
         <v>51</v>
       </c>
       <c r="T9" s="24">
-        <v>16</v>
+        <v>54.956000000000003</v>
       </c>
       <c r="U9" s="22">
         <f>($C$12/T9)*(1/$C$11)*(1/(2*PI()))*60</f>
-        <v>18.780283284843648</v>
+        <v>5.4677293208657538</v>
       </c>
       <c r="W9" s="31">
         <v>1</v>
       </c>
-      <c r="X9" s="33"/>
-      <c r="AK9" s="37"/>
-      <c r="AL9" s="38"/>
-      <c r="AM9" s="38"/>
-      <c r="AN9" s="38"/>
-      <c r="AO9" s="38"/>
-      <c r="AP9" s="39"/>
-      <c r="AS9" s="37"/>
-      <c r="AT9" s="38"/>
-      <c r="AU9" s="38"/>
-      <c r="AV9" s="38"/>
-      <c r="AW9" s="38"/>
-      <c r="AX9" s="39"/>
+      <c r="X9" s="33">
+        <v>6.7629999999999999</v>
+      </c>
+      <c r="AK9" s="52"/>
+      <c r="AL9" s="53"/>
+      <c r="AM9" s="53"/>
+      <c r="AN9" s="53"/>
+      <c r="AO9" s="53"/>
+      <c r="AP9" s="54"/>
+      <c r="AS9" s="52"/>
+      <c r="AT9" s="53"/>
+      <c r="AU9" s="53"/>
+      <c r="AV9" s="53"/>
+      <c r="AW9" s="53"/>
+      <c r="AX9" s="54"/>
     </row>
     <row r="10" spans="1:50" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="B10" s="47" t="s">
+      <c r="B10" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="C10" s="48"/>
+      <c r="C10" s="41"/>
       <c r="E10" s="11">
         <v>1</v>
       </c>
@@ -3160,28 +3169,30 @@
         <v>102</v>
       </c>
       <c r="T10" s="4">
-        <v>7</v>
+        <v>11.531000000000001</v>
       </c>
       <c r="U10" s="15">
         <f>($C$12/T10)*(1/$C$11)*(1/(2*PI()))*60</f>
-        <v>42.926361793928344</v>
+        <v>26.058844207570754</v>
       </c>
       <c r="W10" s="19">
         <v>2</v>
       </c>
-      <c r="X10" s="13"/>
-      <c r="AK10" s="40"/>
-      <c r="AL10" s="41"/>
-      <c r="AM10" s="41"/>
-      <c r="AN10" s="41"/>
-      <c r="AO10" s="41"/>
-      <c r="AP10" s="42"/>
-      <c r="AS10" s="40"/>
-      <c r="AT10" s="41"/>
-      <c r="AU10" s="41"/>
-      <c r="AV10" s="41"/>
-      <c r="AW10" s="41"/>
-      <c r="AX10" s="42"/>
+      <c r="X10" s="13">
+        <v>6.81</v>
+      </c>
+      <c r="AK10" s="55"/>
+      <c r="AL10" s="56"/>
+      <c r="AM10" s="56"/>
+      <c r="AN10" s="56"/>
+      <c r="AO10" s="56"/>
+      <c r="AP10" s="57"/>
+      <c r="AS10" s="55"/>
+      <c r="AT10" s="56"/>
+      <c r="AU10" s="56"/>
+      <c r="AV10" s="56"/>
+      <c r="AW10" s="56"/>
+      <c r="AX10" s="57"/>
     </row>
     <row r="11" spans="1:50" x14ac:dyDescent="0.55000000000000004">
       <c r="B11" s="1" t="s">
@@ -3243,16 +3254,18 @@
         <v>153</v>
       </c>
       <c r="T11" s="4">
-        <v>4</v>
+        <v>7.54</v>
       </c>
       <c r="U11" s="15">
         <f>($C$12/T11)*(1/$C$11)*(1/(2*PI()))*60</f>
-        <v>75.121133139374592</v>
+        <v>39.852060020888388</v>
       </c>
       <c r="W11" s="19">
         <v>3</v>
       </c>
-      <c r="X11" s="13"/>
+      <c r="X11" s="13">
+        <v>6.85</v>
+      </c>
     </row>
     <row r="12" spans="1:50" x14ac:dyDescent="0.55000000000000004">
       <c r="B12" s="1" t="s">
@@ -3314,16 +3327,18 @@
         <v>204</v>
       </c>
       <c r="T12" s="4">
-        <v>2.75</v>
+        <v>6.2450000000000001</v>
       </c>
       <c r="U12" s="15">
         <f>($C$12/T12)*(1/$C$11)*(1/(2*PI()))*60</f>
-        <v>109.26710274818124</v>
+        <v>48.116018023618636</v>
       </c>
       <c r="W12" s="19">
         <v>4</v>
       </c>
-      <c r="X12" s="13"/>
+      <c r="X12" s="13">
+        <v>6.6660000000000004</v>
+      </c>
     </row>
     <row r="13" spans="1:50" x14ac:dyDescent="0.55000000000000004">
       <c r="B13" s="2" t="s">
@@ -3384,16 +3399,18 @@
         <v>255</v>
       </c>
       <c r="T13" s="5">
-        <v>2</v>
+        <v>4.915</v>
       </c>
       <c r="U13" s="17">
         <f>($C$12/T13)*(1/$C$11)*(1/(2*PI()))*60</f>
-        <v>150.24226627874918</v>
+        <v>61.136222290437118</v>
       </c>
       <c r="W13" s="19">
         <v>5</v>
       </c>
-      <c r="X13" s="13"/>
+      <c r="X13" s="13">
+        <v>6.8760000000000003</v>
+      </c>
     </row>
     <row r="14" spans="1:50" x14ac:dyDescent="0.55000000000000004">
       <c r="E14" s="11">
@@ -3447,7 +3464,9 @@
       <c r="W14" s="19">
         <v>6</v>
       </c>
-      <c r="X14" s="13"/>
+      <c r="X14" s="13">
+        <v>6.6429999999999998</v>
+      </c>
     </row>
     <row r="15" spans="1:50" x14ac:dyDescent="0.55000000000000004">
       <c r="E15" s="11">
@@ -3501,7 +3520,9 @@
       <c r="W15" s="19">
         <v>7</v>
       </c>
-      <c r="X15" s="13"/>
+      <c r="X15" s="13">
+        <v>6.8760000000000003</v>
+      </c>
     </row>
     <row r="16" spans="1:50" x14ac:dyDescent="0.55000000000000004">
       <c r="E16" s="11">
@@ -3555,7 +3576,9 @@
       <c r="W16" s="19">
         <v>8</v>
       </c>
-      <c r="X16" s="13"/>
+      <c r="X16" s="13">
+        <v>6.5789999999999997</v>
+      </c>
     </row>
     <row r="17" spans="5:50" ht="14.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="E17" s="11">
@@ -3609,7 +3632,9 @@
       <c r="W17" s="19">
         <v>9</v>
       </c>
-      <c r="X17" s="13"/>
+      <c r="X17" s="13">
+        <v>6.694</v>
+      </c>
     </row>
     <row r="18" spans="5:50" x14ac:dyDescent="0.55000000000000004">
       <c r="E18" s="11">
@@ -3663,7 +3688,9 @@
       <c r="W18" s="32">
         <v>10</v>
       </c>
-      <c r="X18" s="14"/>
+      <c r="X18" s="14">
+        <v>6.6040000000000001</v>
+      </c>
     </row>
     <row r="19" spans="5:50" x14ac:dyDescent="0.55000000000000004">
       <c r="E19" s="12">
@@ -3766,101 +3793,101 @@
       </c>
     </row>
     <row r="21" spans="5:50" x14ac:dyDescent="0.55000000000000004">
-      <c r="E21" s="56">
+      <c r="E21" s="34">
         <v>12</v>
       </c>
-      <c r="F21" s="57">
+      <c r="F21" s="35">
         <v>34.880000000000003</v>
       </c>
-      <c r="G21" s="56">
+      <c r="G21" s="34">
         <v>318.18</v>
       </c>
-      <c r="H21" s="58">
+      <c r="H21" s="36">
         <v>1.72</v>
       </c>
-      <c r="I21" s="59">
+      <c r="I21" s="37">
         <f t="shared" si="9"/>
         <v>1.6915137614678898E-2</v>
       </c>
-      <c r="J21" s="59">
+      <c r="J21" s="37">
         <f t="shared" si="10"/>
         <v>0.90214067278287458</v>
       </c>
-      <c r="K21" s="60">
+      <c r="K21" s="38">
         <f t="shared" si="11"/>
         <v>8.6148088462585548</v>
       </c>
-      <c r="L21" s="59">
+      <c r="L21" s="37">
         <f>E21*$C$13</f>
         <v>0.504</v>
       </c>
-      <c r="M21" s="59">
+      <c r="M21" s="37">
         <f t="shared" si="12"/>
         <v>4.9442400000000006</v>
       </c>
-      <c r="N21" s="59">
+      <c r="N21" s="37">
         <f t="shared" si="13"/>
         <v>92.70450000000001</v>
       </c>
-      <c r="O21" s="60">
+      <c r="O21" s="38">
         <f t="shared" si="14"/>
         <v>547.26959999999997</v>
       </c>
-      <c r="P21" s="60">
+      <c r="P21" s="38">
         <f t="shared" si="15"/>
         <v>83.632500000000007</v>
       </c>
-      <c r="Q21" s="61">
+      <c r="Q21" s="3">
         <f t="shared" si="16"/>
         <v>15.281773370930892</v>
       </c>
     </row>
     <row r="22" spans="5:50" x14ac:dyDescent="0.55000000000000004">
-      <c r="E22" s="56">
+      <c r="E22" s="34">
         <v>13</v>
       </c>
-      <c r="F22" s="57" t="s">
+      <c r="F22" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="G22" s="56">
+      <c r="G22" s="34">
         <v>489.25</v>
       </c>
-      <c r="H22" s="58">
+      <c r="H22" s="36">
         <v>0</v>
       </c>
-      <c r="I22" s="59" t="e">
+      <c r="I22" s="37" t="e">
         <f t="shared" ref="I22" si="17">$C$12/F22</f>
         <v>#VALUE!</v>
       </c>
-      <c r="J22" s="59" t="e">
+      <c r="J22" s="37" t="e">
         <f t="shared" ref="J22" si="18">I22/$C$11</f>
         <v>#VALUE!</v>
       </c>
-      <c r="K22" s="60" t="e">
+      <c r="K22" s="38" t="e">
         <f t="shared" ref="K22" si="19">J22*(1/(2*PI()))*60</f>
         <v>#VALUE!</v>
       </c>
-      <c r="L22" s="59">
+      <c r="L22" s="37">
         <f>E22*$C$13</f>
         <v>0.54600000000000004</v>
       </c>
-      <c r="M22" s="59">
+      <c r="M22" s="37">
         <f t="shared" ref="M22" si="20">L22*9.81</f>
         <v>5.3562600000000007</v>
       </c>
-      <c r="N22" s="59">
+      <c r="N22" s="37">
         <f t="shared" ref="N22" si="21">M22*$C$11*1000</f>
         <v>100.42987500000001</v>
       </c>
-      <c r="O22" s="60">
+      <c r="O22" s="38">
         <f t="shared" ref="O22" si="22">H22*G22</f>
         <v>0</v>
       </c>
-      <c r="P22" s="60" t="e">
+      <c r="P22" s="38" t="e">
         <f t="shared" ref="P22" si="23">J22*N22</f>
         <v>#VALUE!</v>
       </c>
-      <c r="Q22" s="61" t="e">
+      <c r="Q22" s="3" t="e">
         <f t="shared" ref="Q22" si="24">P22/O22*100</f>
         <v>#VALUE!</v>
       </c>
@@ -3870,56 +3897,59 @@
       <c r="K23" t="s">
         <v>41</v>
       </c>
+      <c r="W23" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="24" spans="5:50" ht="14.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="E24" s="47" t="s">
+      <c r="E24" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="F24" s="49"/>
-      <c r="G24" s="49"/>
-      <c r="H24" s="49"/>
-      <c r="I24" s="49"/>
-      <c r="J24" s="49"/>
-      <c r="K24" s="49"/>
-      <c r="L24" s="49"/>
-      <c r="M24" s="49"/>
-      <c r="N24" s="49"/>
-      <c r="O24" s="49"/>
-      <c r="P24" s="49"/>
-      <c r="Q24" s="48"/>
-      <c r="S24" s="43" t="s">
+      <c r="F24" s="42"/>
+      <c r="G24" s="42"/>
+      <c r="H24" s="42"/>
+      <c r="I24" s="42"/>
+      <c r="J24" s="42"/>
+      <c r="K24" s="42"/>
+      <c r="L24" s="42"/>
+      <c r="M24" s="42"/>
+      <c r="N24" s="42"/>
+      <c r="O24" s="42"/>
+      <c r="P24" s="42"/>
+      <c r="Q24" s="41"/>
+      <c r="S24" s="58" t="s">
         <v>25</v>
       </c>
-      <c r="T24" s="45"/>
-      <c r="U24" s="44"/>
-      <c r="W24" s="43" t="s">
+      <c r="T24" s="60"/>
+      <c r="U24" s="59"/>
+      <c r="W24" s="58" t="s">
         <v>30</v>
       </c>
-      <c r="X24" s="44"/>
-      <c r="Z24" s="34" t="s">
+      <c r="X24" s="59"/>
+      <c r="Z24" s="49" t="s">
         <v>20</v>
       </c>
-      <c r="AA24" s="35"/>
-      <c r="AB24" s="35"/>
-      <c r="AC24" s="35"/>
-      <c r="AD24" s="35"/>
-      <c r="AE24" s="36"/>
-      <c r="AK24" s="34" t="s">
+      <c r="AA24" s="50"/>
+      <c r="AB24" s="50"/>
+      <c r="AC24" s="50"/>
+      <c r="AD24" s="50"/>
+      <c r="AE24" s="51"/>
+      <c r="AK24" s="49" t="s">
         <v>18</v>
       </c>
-      <c r="AL24" s="35"/>
-      <c r="AM24" s="35"/>
-      <c r="AN24" s="35"/>
-      <c r="AO24" s="35"/>
-      <c r="AP24" s="36"/>
-      <c r="AS24" s="34" t="s">
+      <c r="AL24" s="50"/>
+      <c r="AM24" s="50"/>
+      <c r="AN24" s="50"/>
+      <c r="AO24" s="50"/>
+      <c r="AP24" s="51"/>
+      <c r="AS24" s="49" t="s">
         <v>19</v>
       </c>
-      <c r="AT24" s="35"/>
-      <c r="AU24" s="35"/>
-      <c r="AV24" s="35"/>
-      <c r="AW24" s="35"/>
-      <c r="AX24" s="36"/>
+      <c r="AT24" s="50"/>
+      <c r="AU24" s="50"/>
+      <c r="AV24" s="50"/>
+      <c r="AW24" s="50"/>
+      <c r="AX24" s="51"/>
     </row>
     <row r="25" spans="5:50" ht="14.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="E25" s="10" t="s">
@@ -3976,26 +4006,26 @@
       <c r="X25" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="Z25" s="37"/>
-      <c r="AA25" s="38"/>
-      <c r="AB25" s="38"/>
-      <c r="AC25" s="38"/>
-      <c r="AD25" s="38"/>
-      <c r="AE25" s="39"/>
-      <c r="AK25" s="37"/>
-      <c r="AL25" s="38"/>
-      <c r="AM25" s="38"/>
-      <c r="AN25" s="38"/>
-      <c r="AO25" s="38"/>
-      <c r="AP25" s="39"/>
-      <c r="AS25" s="37"/>
-      <c r="AT25" s="38"/>
-      <c r="AU25" s="38"/>
-      <c r="AV25" s="38"/>
-      <c r="AW25" s="38"/>
-      <c r="AX25" s="39"/>
+      <c r="Z25" s="52"/>
+      <c r="AA25" s="53"/>
+      <c r="AB25" s="53"/>
+      <c r="AC25" s="53"/>
+      <c r="AD25" s="53"/>
+      <c r="AE25" s="54"/>
+      <c r="AK25" s="52"/>
+      <c r="AL25" s="53"/>
+      <c r="AM25" s="53"/>
+      <c r="AN25" s="53"/>
+      <c r="AO25" s="53"/>
+      <c r="AP25" s="54"/>
+      <c r="AS25" s="52"/>
+      <c r="AT25" s="53"/>
+      <c r="AU25" s="53"/>
+      <c r="AV25" s="53"/>
+      <c r="AW25" s="53"/>
+      <c r="AX25" s="54"/>
     </row>
-    <row r="26" spans="5:50" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="26" spans="5:50" ht="14.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="E26" s="11">
         <v>0</v>
       </c>
@@ -4048,36 +4078,34 @@
         <v>51</v>
       </c>
       <c r="T26" s="24">
-        <v>7</v>
+        <v>21.241</v>
       </c>
       <c r="U26" s="22">
         <f>(($C$12/T26)/$C$11)/(2*3.141)*60</f>
-        <v>42.934461272570154</v>
-      </c>
-      <c r="W26" s="31">
-        <v>1</v>
-      </c>
-      <c r="X26" s="33"/>
-      <c r="Z26" s="40"/>
-      <c r="AA26" s="41"/>
-      <c r="AB26" s="41"/>
-      <c r="AC26" s="41"/>
-      <c r="AD26" s="41"/>
-      <c r="AE26" s="42"/>
-      <c r="AK26" s="40"/>
-      <c r="AL26" s="41"/>
-      <c r="AM26" s="41"/>
-      <c r="AN26" s="41"/>
-      <c r="AO26" s="41"/>
-      <c r="AP26" s="42"/>
-      <c r="AS26" s="40"/>
-      <c r="AT26" s="41"/>
-      <c r="AU26" s="41"/>
-      <c r="AV26" s="41"/>
-      <c r="AW26" s="41"/>
-      <c r="AX26" s="42"/>
+        <v>14.14910921839796</v>
+      </c>
+      <c r="W26" s="19"/>
+      <c r="X26" s="22"/>
+      <c r="Z26" s="52"/>
+      <c r="AA26" s="53"/>
+      <c r="AB26" s="53"/>
+      <c r="AC26" s="53"/>
+      <c r="AD26" s="53"/>
+      <c r="AE26" s="54"/>
+      <c r="AK26" s="52"/>
+      <c r="AL26" s="53"/>
+      <c r="AM26" s="53"/>
+      <c r="AN26" s="53"/>
+      <c r="AO26" s="53"/>
+      <c r="AP26" s="54"/>
+      <c r="AS26" s="52"/>
+      <c r="AT26" s="53"/>
+      <c r="AU26" s="53"/>
+      <c r="AV26" s="53"/>
+      <c r="AW26" s="53"/>
+      <c r="AX26" s="54"/>
     </row>
-    <row r="27" spans="5:50" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="5:50" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="E27" s="11">
         <v>1</v>
       </c>
@@ -4091,56 +4119,76 @@
         <v>3.8</v>
       </c>
       <c r="I27" s="15">
-        <f t="shared" ref="I27:I35" si="25">$C$12/F27</f>
+        <f>$C$12/F27</f>
         <v>0.17307128190085069</v>
       </c>
       <c r="J27" s="15">
-        <f t="shared" ref="J27:J35" si="26">I27/$C$11</f>
+        <f>I27/$C$11</f>
         <v>9.2304683680453703</v>
       </c>
       <c r="K27" s="16">
-        <f t="shared" ref="K27:K35" si="27">J27*(1/(2*PI()))*60</f>
+        <f>J27*(1/(2*PI()))*60</f>
         <v>88.144480069668063</v>
       </c>
       <c r="L27" s="25">
-        <f t="shared" ref="L27:L35" si="28">E27*$C$13</f>
+        <f>E27*$C$13</f>
         <v>4.2000000000000003E-2</v>
       </c>
       <c r="M27" s="25">
-        <f t="shared" ref="M27:M35" si="29">L27*9.81</f>
+        <f>L27*9.81</f>
         <v>0.41202000000000005</v>
       </c>
       <c r="N27" s="15">
-        <f t="shared" ref="N27:N35" si="30">M27*$C$11*1000</f>
+        <f t="shared" ref="N27:N35" si="25">M27*$C$11*1000</f>
         <v>7.7253750000000005</v>
       </c>
       <c r="O27" s="26">
-        <f t="shared" ref="O27:O35" si="31">H27*G27</f>
+        <f>H27*G27</f>
         <v>447.60199999999998</v>
       </c>
       <c r="P27" s="16">
-        <f t="shared" ref="P27:P35" si="32">J27*N27</f>
+        <f>J27*N27</f>
         <v>71.308829568788511</v>
       </c>
       <c r="Q27" s="6">
-        <f t="shared" ref="Q27:Q35" si="33">P27/O27*100</f>
+        <f>P27/O27*100</f>
         <v>15.931302712853945</v>
       </c>
-      <c r="S27" s="20">
-        <f>255*0.6</f>
-        <v>153</v>
-      </c>
-      <c r="T27" s="4">
-        <v>1.8</v>
-      </c>
-      <c r="U27" s="15">
+      <c r="S27" s="23">
+        <f>255*0.4</f>
+        <v>102</v>
+      </c>
+      <c r="T27" s="24">
+        <v>7.9279999999999999</v>
+      </c>
+      <c r="U27" s="22">
         <f>(($C$12/T27)/$C$11)/(2*3.141)*60</f>
-        <v>166.96734939332836</v>
-      </c>
-      <c r="W27" s="19">
-        <v>3</v>
-      </c>
-      <c r="X27" s="13"/>
+        <v>37.908833111502403</v>
+      </c>
+      <c r="W27" s="31">
+        <v>1</v>
+      </c>
+      <c r="X27" s="33">
+        <v>5.9889999999999999</v>
+      </c>
+      <c r="Z27" s="55"/>
+      <c r="AA27" s="56"/>
+      <c r="AB27" s="56"/>
+      <c r="AC27" s="56"/>
+      <c r="AD27" s="56"/>
+      <c r="AE27" s="57"/>
+      <c r="AK27" s="55"/>
+      <c r="AL27" s="56"/>
+      <c r="AM27" s="56"/>
+      <c r="AN27" s="56"/>
+      <c r="AO27" s="56"/>
+      <c r="AP27" s="57"/>
+      <c r="AS27" s="55"/>
+      <c r="AT27" s="56"/>
+      <c r="AU27" s="56"/>
+      <c r="AV27" s="56"/>
+      <c r="AW27" s="56"/>
+      <c r="AX27" s="57"/>
     </row>
     <row r="28" spans="5:50" x14ac:dyDescent="0.55000000000000004">
       <c r="E28" s="11">
@@ -4156,56 +4204,58 @@
         <v>3.36</v>
       </c>
       <c r="I28" s="15">
+        <f>$C$12/F28</f>
+        <v>0.15344603381014302</v>
+      </c>
+      <c r="J28" s="15">
+        <f>I28/$C$11</f>
+        <v>8.183788469874294</v>
+      </c>
+      <c r="K28" s="16">
+        <f>J28*(1/(2*PI()))*60</f>
+        <v>78.149423291937154</v>
+      </c>
+      <c r="L28" s="25">
+        <f>E28*$C$13</f>
+        <v>8.4000000000000005E-2</v>
+      </c>
+      <c r="M28" s="25">
+        <f>L28*9.81</f>
+        <v>0.82404000000000011</v>
+      </c>
+      <c r="N28" s="15">
         <f t="shared" si="25"/>
-        <v>0.15344603381014302</v>
-      </c>
-      <c r="J28" s="15">
-        <f t="shared" si="26"/>
-        <v>8.183788469874294</v>
-      </c>
-      <c r="K28" s="16">
-        <f t="shared" si="27"/>
-        <v>78.149423291937154</v>
-      </c>
-      <c r="L28" s="25">
-        <f t="shared" si="28"/>
-        <v>8.4000000000000005E-2</v>
-      </c>
-      <c r="M28" s="25">
-        <f t="shared" si="29"/>
-        <v>0.82404000000000011</v>
-      </c>
-      <c r="N28" s="15">
-        <f t="shared" si="30"/>
         <v>15.450750000000001</v>
       </c>
       <c r="O28" s="26">
-        <f t="shared" si="31"/>
+        <f>H28*G28</f>
         <v>536.99519999999995</v>
       </c>
       <c r="P28" s="16">
-        <f t="shared" si="32"/>
+        <f>J28*N28</f>
         <v>126.44566970091026</v>
       </c>
       <c r="Q28" s="6">
-        <f t="shared" si="33"/>
+        <f>P28/O28*100</f>
         <v>23.546890121347502</v>
       </c>
       <c r="S28" s="20">
-        <f>255*0.8</f>
-        <v>204</v>
+        <f>255*0.6</f>
+        <v>153</v>
       </c>
       <c r="T28" s="4">
-        <v>1.4</v>
+        <v>5.5110000000000001</v>
       </c>
       <c r="U28" s="15">
         <f>(($C$12/T28)/$C$11)/(2*3.141)*60</f>
-        <v>214.67230636285078</v>
+        <v>54.534790221010894</v>
       </c>
       <c r="W28" s="19">
-        <v>4</v>
-      </c>
-      <c r="X28" s="13"/>
+        <v>2</v>
+      </c>
+      <c r="X28" s="13">
+        <v>5.6630000000000003</v>
+      </c>
     </row>
     <row r="29" spans="5:50" x14ac:dyDescent="0.55000000000000004">
       <c r="E29" s="11">
@@ -4225,51 +4275,54 @@
         <v>0.13055985837574682</v>
       </c>
       <c r="J29" s="15">
-        <f t="shared" si="26"/>
+        <f>I29/$C$11</f>
         <v>6.9631924467064978</v>
       </c>
       <c r="K29" s="16">
-        <f t="shared" si="27"/>
+        <f>J29*(1/(2*PI()))*60</f>
         <v>66.493589855609287</v>
       </c>
       <c r="L29" s="25">
-        <f t="shared" si="28"/>
+        <f>E29*$C$13</f>
         <v>0.126</v>
       </c>
       <c r="M29" s="25">
-        <f t="shared" si="29"/>
+        <f>L29*9.81</f>
         <v>1.2360600000000002</v>
       </c>
       <c r="N29" s="15">
-        <f t="shared" si="30"/>
+        <f t="shared" si="25"/>
         <v>23.176125000000003</v>
       </c>
       <c r="O29" s="26">
-        <f t="shared" si="31"/>
+        <f>H29*G29</f>
         <v>577.29960000000005</v>
       </c>
       <c r="P29" s="16">
-        <f t="shared" si="32"/>
+        <f>J29*N29</f>
         <v>161.37981854392564</v>
       </c>
       <c r="Q29" s="6">
-        <f t="shared" si="33"/>
+        <f>P29/O29*100</f>
         <v>27.954257814127299</v>
       </c>
-      <c r="S29" s="21">
-        <v>255</v>
-      </c>
-      <c r="T29" s="5">
-        <v>1</v>
-      </c>
-      <c r="U29" s="17">
+      <c r="S29" s="20">
+        <f>255*0.8</f>
+        <v>204</v>
+      </c>
+      <c r="T29" s="4">
+        <v>4.5730000000000004</v>
+      </c>
+      <c r="U29" s="15">
         <f>(($C$12/T29)/$C$11)/(2*3.141)*60</f>
-        <v>300.54122890799107</v>
+        <v>65.72080229783316</v>
       </c>
       <c r="W29" s="19">
-        <v>5</v>
-      </c>
-      <c r="X29" s="13"/>
+        <v>3</v>
+      </c>
+      <c r="X29" s="13">
+        <v>5.77</v>
+      </c>
     </row>
     <row r="30" spans="5:50" x14ac:dyDescent="0.55000000000000004">
       <c r="E30" s="11">
@@ -4289,41 +4342,53 @@
         <v>0.10940107546819952</v>
       </c>
       <c r="J30" s="15">
-        <f t="shared" si="26"/>
+        <f>I30/$C$11</f>
         <v>5.8347240249706411</v>
       </c>
       <c r="K30" s="16">
-        <f t="shared" si="27"/>
+        <f>J30*(1/(2*PI()))*60</f>
         <v>55.717510209067015</v>
       </c>
       <c r="L30" s="25">
-        <f t="shared" si="28"/>
+        <f>E30*$C$13</f>
         <v>0.16800000000000001</v>
       </c>
       <c r="M30" s="25">
-        <f t="shared" si="29"/>
+        <f>L30*9.81</f>
         <v>1.6480800000000002</v>
       </c>
       <c r="N30" s="15">
-        <f t="shared" si="30"/>
+        <f t="shared" si="25"/>
         <v>30.901500000000002</v>
       </c>
       <c r="O30" s="26">
-        <f t="shared" si="31"/>
+        <f>H30*G30</f>
         <v>601.56479999999999</v>
       </c>
       <c r="P30" s="16">
-        <f t="shared" si="32"/>
+        <f>J30*N30</f>
         <v>180.30172445763029</v>
       </c>
       <c r="Q30" s="6">
-        <f t="shared" si="33"/>
+        <f>P30/O30*100</f>
         <v>29.972120120331226</v>
       </c>
+      <c r="S30" s="21">
+        <v>255</v>
+      </c>
+      <c r="T30" s="5">
+        <v>3.78</v>
+      </c>
+      <c r="U30" s="17">
+        <f>(($C$12/T30)/$C$11)/(2*3.141)*60</f>
+        <v>79.508261615870651</v>
+      </c>
       <c r="W30" s="19">
-        <v>6</v>
-      </c>
-      <c r="X30" s="13"/>
+        <v>4</v>
+      </c>
+      <c r="X30" s="13">
+        <v>5.8230000000000004</v>
+      </c>
     </row>
     <row r="31" spans="5:50" x14ac:dyDescent="0.55000000000000004">
       <c r="E31" s="11">
@@ -4339,45 +4404,47 @@
         <v>2.4900000000000002</v>
       </c>
       <c r="I31" s="15">
+        <f>$C$12/F31</f>
+        <v>8.9870525514089861E-2</v>
+      </c>
+      <c r="J31" s="15">
+        <f>I31/$C$11</f>
+        <v>4.7930946940847932</v>
+      </c>
+      <c r="K31" s="16">
+        <f>J31*(1/(2*PI()))*60</f>
+        <v>45.770682796267849</v>
+      </c>
+      <c r="L31" s="25">
+        <f>E31*$C$13</f>
+        <v>0.21000000000000002</v>
+      </c>
+      <c r="M31" s="25">
+        <f>L31*9.81</f>
+        <v>2.0601000000000003</v>
+      </c>
+      <c r="N31" s="15">
         <f t="shared" si="25"/>
-        <v>8.9870525514089861E-2</v>
-      </c>
-      <c r="J31" s="15">
-        <f t="shared" si="26"/>
-        <v>4.7930946940847932</v>
-      </c>
-      <c r="K31" s="16">
-        <f t="shared" si="27"/>
-        <v>45.770682796267849</v>
-      </c>
-      <c r="L31" s="25">
-        <f t="shared" si="28"/>
-        <v>0.21000000000000002</v>
-      </c>
-      <c r="M31" s="25">
-        <f t="shared" si="29"/>
-        <v>2.0601000000000003</v>
-      </c>
-      <c r="N31" s="15">
-        <f t="shared" si="30"/>
         <v>38.626875000000005</v>
       </c>
       <c r="O31" s="26">
-        <f t="shared" si="31"/>
+        <f>H31*G31</f>
         <v>606.06600000000003</v>
       </c>
       <c r="P31" s="16">
-        <f t="shared" si="32"/>
+        <f>J31*N31</f>
         <v>185.14226961157658</v>
       </c>
       <c r="Q31" s="6">
-        <f t="shared" si="33"/>
+        <f>P31/O31*100</f>
         <v>30.548202606906933</v>
       </c>
       <c r="W31" s="19">
-        <v>7</v>
-      </c>
-      <c r="X31" s="13"/>
+        <v>5</v>
+      </c>
+      <c r="X31" s="13">
+        <v>5.952</v>
+      </c>
     </row>
     <row r="32" spans="5:50" x14ac:dyDescent="0.55000000000000004">
       <c r="E32" s="11">
@@ -4393,45 +4460,47 @@
         <v>2.1800000000000002</v>
       </c>
       <c r="I32" s="15">
+        <f>$C$12/F32</f>
+        <v>7.6822916666666671E-2</v>
+      </c>
+      <c r="J32" s="15">
+        <f>I32/$C$11</f>
+        <v>4.0972222222222223</v>
+      </c>
+      <c r="K32" s="16">
+        <f>J32*(1/(2*PI()))*60</f>
+        <v>39.125590176757605</v>
+      </c>
+      <c r="L32" s="25">
+        <f>E32*$C$13</f>
+        <v>0.252</v>
+      </c>
+      <c r="M32" s="25">
+        <f>L32*9.81</f>
+        <v>2.4721200000000003</v>
+      </c>
+      <c r="N32" s="15">
         <f t="shared" si="25"/>
-        <v>7.6822916666666671E-2</v>
-      </c>
-      <c r="J32" s="15">
-        <f t="shared" si="26"/>
-        <v>4.0972222222222223</v>
-      </c>
-      <c r="K32" s="16">
-        <f t="shared" si="27"/>
-        <v>39.125590176757605</v>
-      </c>
-      <c r="L32" s="25">
-        <f t="shared" si="28"/>
-        <v>0.252</v>
-      </c>
-      <c r="M32" s="25">
-        <f t="shared" si="29"/>
-        <v>2.4721200000000003</v>
-      </c>
-      <c r="N32" s="15">
-        <f t="shared" si="30"/>
         <v>46.352250000000005</v>
       </c>
       <c r="O32" s="26">
-        <f t="shared" si="31"/>
+        <f>H32*G32</f>
         <v>595.6196000000001</v>
       </c>
       <c r="P32" s="16">
-        <f t="shared" si="32"/>
+        <f>J32*N32</f>
         <v>189.91546875000003</v>
       </c>
       <c r="Q32" s="6">
-        <f t="shared" si="33"/>
+        <f>P32/O32*100</f>
         <v>31.88536252836542</v>
       </c>
       <c r="W32" s="19">
-        <v>8</v>
-      </c>
-      <c r="X32" s="13"/>
+        <v>6</v>
+      </c>
+      <c r="X32" s="13">
+        <v>5.7350000000000003</v>
+      </c>
     </row>
     <row r="33" spans="5:24" x14ac:dyDescent="0.55000000000000004">
       <c r="E33" s="11">
@@ -4447,45 +4516,47 @@
         <v>2.11</v>
       </c>
       <c r="I33" s="15">
+        <f>$C$12/F33</f>
+        <v>5.5456339881567819E-2</v>
+      </c>
+      <c r="J33" s="15">
+        <f>I33/$C$11</f>
+        <v>2.9576714603502836</v>
+      </c>
+      <c r="K33" s="16">
+        <f>J33*(1/(2*PI()))*60</f>
+        <v>28.243681977394345</v>
+      </c>
+      <c r="L33" s="25">
+        <f>E33*$C$13</f>
+        <v>0.29400000000000004</v>
+      </c>
+      <c r="M33" s="25">
+        <f>L33*9.81</f>
+        <v>2.8841400000000004</v>
+      </c>
+      <c r="N33" s="15">
         <f t="shared" si="25"/>
-        <v>5.5456339881567819E-2</v>
-      </c>
-      <c r="J33" s="15">
-        <f t="shared" si="26"/>
-        <v>2.9576714603502836</v>
-      </c>
-      <c r="K33" s="16">
-        <f t="shared" si="27"/>
-        <v>28.243681977394345</v>
-      </c>
-      <c r="L33" s="25">
-        <f t="shared" si="28"/>
-        <v>0.29400000000000004</v>
-      </c>
-      <c r="M33" s="25">
-        <f t="shared" si="29"/>
-        <v>2.8841400000000004</v>
-      </c>
-      <c r="N33" s="15">
-        <f t="shared" si="30"/>
         <v>54.077625000000005</v>
       </c>
       <c r="O33" s="26">
-        <f t="shared" si="31"/>
+        <f>H33*G33</f>
         <v>594.0071999999999</v>
       </c>
       <c r="P33" s="16">
-        <f t="shared" si="32"/>
+        <f>J33*N33</f>
         <v>159.94384810602503</v>
       </c>
       <c r="Q33" s="6">
-        <f t="shared" si="33"/>
+        <f>P33/O33*100</f>
         <v>26.926247376466993</v>
       </c>
       <c r="W33" s="19">
-        <v>9</v>
-      </c>
-      <c r="X33" s="13"/>
+        <v>7</v>
+      </c>
+      <c r="X33" s="13">
+        <v>5.6609999999999996</v>
+      </c>
     </row>
     <row r="34" spans="5:24" x14ac:dyDescent="0.55000000000000004">
       <c r="E34" s="11">
@@ -4501,45 +4572,47 @@
         <v>1.59</v>
       </c>
       <c r="I34" s="15">
+        <f>$C$12/F34</f>
+        <v>3.6415257375632636E-2</v>
+      </c>
+      <c r="J34" s="15">
+        <f>I34/$C$11</f>
+        <v>1.9421470600337407</v>
+      </c>
+      <c r="K34" s="16">
+        <f>J34*(1/(2*PI()))*60</f>
+        <v>18.546138288945709</v>
+      </c>
+      <c r="L34" s="25">
+        <f>E34*$C$13</f>
+        <v>0.33600000000000002</v>
+      </c>
+      <c r="M34" s="25">
+        <f>L34*9.81</f>
+        <v>3.2961600000000004</v>
+      </c>
+      <c r="N34" s="15">
         <f t="shared" si="25"/>
-        <v>3.6415257375632636E-2</v>
-      </c>
-      <c r="J34" s="15">
-        <f t="shared" si="26"/>
-        <v>1.9421470600337407</v>
-      </c>
-      <c r="K34" s="16">
-        <f t="shared" si="27"/>
-        <v>18.546138288945709</v>
-      </c>
-      <c r="L34" s="25">
-        <f t="shared" si="28"/>
-        <v>0.33600000000000002</v>
-      </c>
-      <c r="M34" s="25">
-        <f t="shared" si="29"/>
-        <v>3.2961600000000004</v>
-      </c>
-      <c r="N34" s="15">
-        <f t="shared" si="30"/>
         <v>61.803000000000004</v>
       </c>
       <c r="O34" s="26">
-        <f t="shared" si="31"/>
+        <f>H34*G34</f>
         <v>528.45240000000001</v>
       </c>
       <c r="P34" s="16">
-        <f t="shared" si="32"/>
+        <f>J34*N34</f>
         <v>120.03051475126529</v>
       </c>
       <c r="Q34" s="6">
-        <f t="shared" si="33"/>
+        <f>P34/O34*100</f>
         <v>22.713590618807917</v>
       </c>
-      <c r="W34" s="32">
-        <v>10</v>
-      </c>
-      <c r="X34" s="14"/>
+      <c r="W34" s="19">
+        <v>8</v>
+      </c>
+      <c r="X34" s="13">
+        <v>5.57</v>
+      </c>
     </row>
     <row r="35" spans="5:24" x14ac:dyDescent="0.55000000000000004">
       <c r="E35" s="12">
@@ -4555,44 +4628,67 @@
         <v>0</v>
       </c>
       <c r="I35" s="17" t="e">
+        <f>$C$12/F35</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="J35" s="17" t="e">
+        <f>I35/$C$11</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K35" s="18" t="e">
+        <f>J35*(1/(2*PI()))*60</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="L35" s="28">
+        <f>E35*$C$13</f>
+        <v>0.378</v>
+      </c>
+      <c r="M35" s="28">
+        <f>L35*9.81</f>
+        <v>3.70818</v>
+      </c>
+      <c r="N35" s="17">
         <f t="shared" si="25"/>
+        <v>69.528374999999997</v>
+      </c>
+      <c r="O35" s="18">
+        <f>H35*G35</f>
+        <v>0</v>
+      </c>
+      <c r="P35" s="18" t="e">
+        <f>J35*N35</f>
         <v>#VALUE!</v>
       </c>
-      <c r="J35" s="17" t="e">
-        <f t="shared" si="26"/>
+      <c r="Q35" s="9" t="e">
+        <f>P35/O35*100</f>
         <v>#VALUE!</v>
       </c>
-      <c r="K35" s="18" t="e">
-        <f t="shared" si="27"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="L35" s="28">
-        <f t="shared" si="28"/>
-        <v>0.378</v>
-      </c>
-      <c r="M35" s="28">
-        <f t="shared" si="29"/>
-        <v>3.70818</v>
-      </c>
-      <c r="N35" s="17">
-        <f t="shared" si="30"/>
-        <v>69.528374999999997</v>
-      </c>
-      <c r="O35" s="18">
-        <f t="shared" si="31"/>
-        <v>0</v>
-      </c>
-      <c r="P35" s="18" t="e">
-        <f t="shared" si="32"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="Q35" s="9" t="e">
-        <f t="shared" si="33"/>
-        <v>#VALUE!</v>
+      <c r="W35" s="19">
+        <v>9</v>
+      </c>
+      <c r="X35" s="13">
+        <v>5.8070000000000004</v>
+      </c>
+    </row>
+    <row r="36" spans="5:24" x14ac:dyDescent="0.55000000000000004">
+      <c r="W36" s="32">
+        <v>10</v>
+      </c>
+      <c r="X36" s="14">
+        <v>5.6980000000000004</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="Z24:AE27"/>
+    <mergeCell ref="AS24:AX27"/>
+    <mergeCell ref="W7:X7"/>
+    <mergeCell ref="W24:X24"/>
+    <mergeCell ref="S24:U24"/>
+    <mergeCell ref="S7:U7"/>
+    <mergeCell ref="AK8:AP10"/>
+    <mergeCell ref="AS8:AX10"/>
+    <mergeCell ref="AK24:AP27"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A2:E2"/>
     <mergeCell ref="B10:C10"/>
@@ -4602,15 +4698,6 @@
     <mergeCell ref="B6:B8"/>
     <mergeCell ref="P4:V4"/>
     <mergeCell ref="J4:N4"/>
-    <mergeCell ref="Z24:AE26"/>
-    <mergeCell ref="AS24:AX26"/>
-    <mergeCell ref="W7:X7"/>
-    <mergeCell ref="W24:X24"/>
-    <mergeCell ref="S24:U24"/>
-    <mergeCell ref="S7:U7"/>
-    <mergeCell ref="AK8:AP10"/>
-    <mergeCell ref="AS8:AX10"/>
-    <mergeCell ref="AK24:AP26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>